<commit_message>
Tabell baseline med p-verdi
</commit_message>
<xml_diff>
--- a/Baselinekarakteristika/p.value.diff.pre.xlsx
+++ b/Baselinekarakteristika/p.value.diff.pre.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Breili/Documents/HINN/Masteroppgave/1. NY MASTERPROSJEKT/RESULTATER/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Breili/Documents/HINN/Masteroppgave/1. NY MASTERPROSJEKT/RESULTATER/Masteroppgave/Baselinekarakteristika/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E5C7729-9F78-0942-BAA7-E2655D949F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2E5B64-48E3-8246-9CEA-312665C7AAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34280" yWindow="960" windowWidth="27640" windowHeight="16440" xr2:uid="{E12EB877-5062-3346-AFB2-37E3D8D14704}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="10000" windowHeight="17500" xr2:uid="{E12EB877-5062-3346-AFB2-37E3D8D14704}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>p.value</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>variable</t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>p.value.w</t>
+  </si>
+  <si>
+    <t>p.value.m</t>
+  </si>
+  <si>
+    <t>p.value.m.eks</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -447,18 +462,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13CF4F-9EA2-C244-A1D5-A53E148B75DC}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -468,8 +484,17 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -479,8 +504,17 @@
       <c r="C2">
         <v>0.45500000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="E2">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -490,8 +524,17 @@
       <c r="C3">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="E3">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -501,8 +544,17 @@
       <c r="C4">
         <v>3.85E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0.22</v>
+      </c>
+      <c r="E4">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.42299999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -512,8 +564,17 @@
       <c r="C5">
         <v>3.6700000000000003E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="E5">
+        <v>5.9799999999999999E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -523,8 +584,17 @@
       <c r="C6">
         <v>3.27E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="E6">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.32200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -534,8 +604,17 @@
       <c r="C7">
         <v>0.11600000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.248</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -543,10 +622,19 @@
         <v>0.58299999999999996</v>
       </c>
       <c r="C8">
-        <v>0.68600000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="E8">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -556,8 +644,17 @@
       <c r="C9">
         <v>0.219</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -567,8 +664,17 @@
       <c r="C10">
         <v>3.2899999999999999E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="E10">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -578,8 +684,17 @@
       <c r="C11">
         <v>0.622</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="E11">
+        <v>0.68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -589,8 +704,17 @@
       <c r="C12">
         <v>0.1313</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>0.219</v>
+      </c>
+      <c r="E12">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -600,8 +724,17 @@
       <c r="C13">
         <v>6.1800000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="E13">
+        <v>9.5799999999999996E-2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -611,8 +744,17 @@
       <c r="C14">
         <v>0.74099999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>0.435</v>
+      </c>
+      <c r="E14">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -622,8 +764,17 @@
       <c r="C15">
         <v>4.5699999999999998E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>0.221</v>
+      </c>
+      <c r="E15">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -633,8 +784,17 @@
       <c r="C16">
         <v>0.87309999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>0.72</v>
+      </c>
+      <c r="E16">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -644,8 +804,17 @@
       <c r="C17">
         <v>0.876</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>0.879</v>
+      </c>
+      <c r="E17">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -654,6 +823,35 @@
       </c>
       <c r="C18">
         <v>0.51900000000000002</v>
+      </c>
+      <c r="D18">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="C19">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="D19">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tabell 1 1. utkast
</commit_message>
<xml_diff>
--- a/Baselinekarakteristika/p.value.diff.pre.xlsx
+++ b/Baselinekarakteristika/p.value.diff.pre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Breili/Documents/HINN/Masteroppgave/1. NY MASTERPROSJEKT/RESULTATER/Masteroppgave/Baselinekarakteristika/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2E5B64-48E3-8246-9CEA-312665C7AAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDC465C-38B8-C84B-A113-5452A4C929AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="10000" windowHeight="17500" xr2:uid="{E12EB877-5062-3346-AFB2-37E3D8D14704}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>p.value</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13CF4F-9EA2-C244-A1D5-A53E148B75DC}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,39 +499,24 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="C2">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="D2">
-        <v>0.64900000000000002</v>
-      </c>
-      <c r="E2">
-        <v>0.56399999999999995</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0.89200000000000002</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="C3">
-        <v>0.48</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="D3">
-        <v>0.57799999999999996</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="E3">
-        <v>0.67700000000000005</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -536,99 +524,99 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0.105</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="C4">
-        <v>3.85E-2</v>
+        <v>0.48</v>
       </c>
       <c r="D4">
-        <v>0.22</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="E4">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="F4">
-        <v>0.42299999999999999</v>
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>3.32E-2</v>
+        <v>0.105</v>
       </c>
       <c r="C5">
-        <v>3.6700000000000003E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="D5">
-        <v>0.26300000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="E5">
-        <v>5.9799999999999999E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="F5">
-        <v>0.26</v>
+        <v>0.42299999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>1.72E-2</v>
+        <v>3.32E-2</v>
       </c>
       <c r="C6">
-        <v>3.27E-2</v>
+        <v>3.6700000000000003E-2</v>
       </c>
       <c r="D6">
-        <v>0.24299999999999999</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="E6">
-        <v>7.1400000000000005E-2</v>
+        <v>5.9799999999999999E-2</v>
       </c>
       <c r="F6">
-        <v>0.32200000000000001</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>0.72699999999999998</v>
+        <v>1.72E-2</v>
       </c>
       <c r="C7">
-        <v>0.11600000000000001</v>
+        <v>3.27E-2</v>
       </c>
       <c r="D7">
-        <v>0.29199999999999998</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="E7">
-        <v>0.248</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.32200000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>0.58299999999999996</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="C8">
-        <v>0.63800000000000001</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="D8">
-        <v>0.58299999999999996</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="E8">
-        <v>0.23100000000000001</v>
+        <v>0.248</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -636,19 +624,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>0.26700000000000002</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="C9">
-        <v>0.219</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="D9">
-        <v>6.7100000000000007E-2</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="E9">
-        <v>0.96699999999999997</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
@@ -656,59 +644,59 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>7.1599999999999997E-2</v>
+        <v>0.26700000000000002</v>
       </c>
       <c r="C10">
-        <v>3.2899999999999999E-2</v>
+        <v>0.219</v>
       </c>
       <c r="D10">
-        <v>0.35299999999999998</v>
+        <v>6.7100000000000007E-2</v>
       </c>
       <c r="E10">
-        <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="F10">
-        <v>0.12</v>
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>0.57799999999999996</v>
+        <v>7.1599999999999997E-2</v>
       </c>
       <c r="C11">
-        <v>0.622</v>
+        <v>3.2899999999999999E-2</v>
       </c>
       <c r="D11">
-        <v>0.78100000000000003</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="E11">
-        <v>0.68</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>6.1499999999999999E-2</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="C12">
-        <v>0.1313</v>
+        <v>0.622</v>
       </c>
       <c r="D12">
-        <v>0.219</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="E12">
-        <v>0.39600000000000002</v>
+        <v>0.68</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
@@ -716,19 +704,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>0.112</v>
+        <v>6.1499999999999999E-2</v>
       </c>
       <c r="C13">
-        <v>6.1800000000000001E-2</v>
+        <v>0.1313</v>
       </c>
       <c r="D13">
-        <v>0.32400000000000001</v>
+        <v>0.219</v>
       </c>
       <c r="E13">
-        <v>9.5799999999999996E-2</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -736,59 +724,59 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>0.95699999999999996</v>
+        <v>0.112</v>
       </c>
       <c r="C14">
-        <v>0.74099999999999999</v>
+        <v>6.1800000000000001E-2</v>
       </c>
       <c r="D14">
-        <v>0.435</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="E14">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="F14">
-        <v>0.41799999999999998</v>
+        <v>9.5799999999999996E-2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>0.39900000000000002</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="C15">
-        <v>4.5699999999999998E-2</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="D15">
-        <v>0.221</v>
+        <v>0.435</v>
       </c>
       <c r="E15">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="F15" t="s">
-        <v>24</v>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F15">
+        <v>0.41799999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>0.63800000000000001</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="C16">
-        <v>0.87309999999999999</v>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="D16">
-        <v>0.72</v>
+        <v>0.221</v>
       </c>
       <c r="E16">
-        <v>0.61299999999999999</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
@@ -796,19 +784,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>0.77739999999999998</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="C17">
-        <v>0.876</v>
+        <v>0.87309999999999999</v>
       </c>
       <c r="D17">
-        <v>0.879</v>
+        <v>0.72</v>
       </c>
       <c r="E17">
-        <v>0.98199999999999998</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="F17" t="s">
         <v>24</v>
@@ -816,19 +804,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>0.501</v>
+        <v>0.77739999999999998</v>
       </c>
       <c r="C18">
-        <v>0.51900000000000002</v>
+        <v>0.876</v>
       </c>
       <c r="D18">
-        <v>0.45300000000000001</v>
+        <v>0.879</v>
       </c>
       <c r="E18">
-        <v>0.88200000000000001</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
@@ -836,21 +824,41 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.501</v>
+      </c>
+      <c r="C19">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="D19">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>0.24299999999999999</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0.58799999999999997</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>0.61399999999999999</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>0.39600000000000002</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>